<commit_message>
campaign pom class is created
</commit_message>
<xml_diff>
--- a/GUISeleniumFramework/testdata/testScriptdata.xlsx
+++ b/GUISeleniumFramework/testdata/testScriptdata.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20400"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B66EEE0E-7793-4D98-9BEE-A78371A6E345}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nivetha Shanmugam\git\Cronos_Project_Framework\GUISeleniumFramework\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4382B15-DE95-494C-8B3F-EB9A73B600FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11620" windowHeight="6330" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="3" r:id="rId1"/>
     <sheet name="org" sheetId="1" r:id="rId2"/>
     <sheet name="product" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId4"/>
+    <sheet name="CampaignModule" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="150">
   <si>
     <t>TC_ID</t>
   </si>
@@ -444,6 +449,36 @@
   </si>
   <si>
     <t>faceBook_kdd</t>
+  </si>
+  <si>
+    <t>TESTCASENAME</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>CAMPAIGN_NAME</t>
+  </si>
+  <si>
+    <t>EVENT_NAME</t>
+  </si>
+  <si>
+    <t>CreateContactWithEvents</t>
+  </si>
+  <si>
+    <t>GreenLiving</t>
+  </si>
+  <si>
+    <t>BreezyBrights</t>
+  </si>
+  <si>
+    <t>SEARCHTEXTFIELD</t>
+  </si>
+  <si>
+    <t>Tc_02</t>
+  </si>
+  <si>
+    <t>CreateCampaignAndDeletingTheCampaign</t>
   </si>
 </sst>
 </file>
@@ -516,7 +551,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -801,7 +836,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -923,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1103,6 +1138,83 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE9AED9-5CEA-4DF2-8D37-79CE660AF180}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="40.7265625" customWidth="1"/>
+    <col min="3" max="3" width="31.453125" customWidth="1"/>
+    <col min="4" max="4" width="35.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7004AA42-F8FF-45C9-AB36-1F51EDB304F0}">
   <dimension ref="A1:B100"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updates in project framework
</commit_message>
<xml_diff>
--- a/GUISeleniumFramework/testdata/testScriptdata.xlsx
+++ b/GUISeleniumFramework/testdata/testScriptdata.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
-  <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2895EFB1-ACCB-4A1F-B1FB-66AA4763E1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="6075" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="3" r:id="rId1"/>
-    <sheet name="org" sheetId="1" r:id="rId2"/>
-    <sheet name="product" sheetId="4" r:id="rId3"/>
-    <sheet name="ProductModule" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
+    <sheet name="org" sheetId="1" r:id="rId3"/>
+    <sheet name="product" sheetId="4" r:id="rId4"/>
+    <sheet name="ProductModule" sheetId="5" r:id="rId5"/>
+    <sheet name="CampaignModule" sheetId="7" r:id="rId6"/>
+    <sheet name="OpportunitiesModule" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O25"/>
+  <oleSize ref="A1:E18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="165">
   <si>
     <t>TC_ID</t>
   </si>
@@ -475,13 +477,58 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>CampaignName</t>
+  </si>
+  <si>
+    <t>EventName</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>Create campaign with events</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>Search campaign and delete</t>
+  </si>
+  <si>
+    <t>Breezy Brights</t>
+  </si>
+  <si>
+    <t>Greenliving</t>
+  </si>
+  <si>
+    <t>Create opportunity with organization name and assign to group</t>
+  </si>
+  <si>
+    <t>Create opportunity with organization name with back date from current date</t>
+  </si>
+  <si>
+    <t>OrganizationName</t>
+  </si>
+  <si>
+    <t>OpportunityName</t>
+  </si>
+  <si>
+    <t>Expected_Close_Date</t>
+  </si>
+  <si>
+    <t>PIMCHA</t>
+  </si>
+  <si>
+    <t>HempCann</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,8 +536,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,6 +559,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -548,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -556,6 +615,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -835,22 +899,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618505B5-BC18-40DF-B31F-D9D1863412AA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -865,7 +929,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>115</v>
       </c>
@@ -878,14 +942,14 @@
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -900,7 +964,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>116</v>
       </c>
@@ -913,14 +977,14 @@
       <c r="D5" s="3"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -937,7 +1001,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>127</v>
       </c>
@@ -958,21 +1022,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="130" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.77734375" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -985,7 +1061,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -998,7 +1074,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1015,7 +1091,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>110</v>
       </c>
@@ -1032,7 +1108,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +1122,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>111</v>
       </c>
@@ -1060,7 +1136,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1072,7 +1148,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>115</v>
       </c>
@@ -1089,21 +1165,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6E95A9-5958-495C-AC30-1DA708189BFF}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>133</v>
       </c>
@@ -1111,7 +1187,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>135</v>
       </c>
@@ -1119,7 +1195,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>135</v>
       </c>
@@ -1127,83 +1203,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>138</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F43B8C5-95E3-4E18-BB7A-9D98E83EDD1A}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C5">
-        <v>15000</v>
       </c>
     </row>
   </sheetData>
@@ -1212,20 +1217,229 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7004AA42-F8FF-45C9-AB36-1F51EDB304F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5">
+        <v>15000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="8"/>
+    <col min="2" max="2" width="27.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" s="8">
+        <v>45527</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="8">
+        <v>44795</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1233,7 +1447,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1241,7 +1455,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1249,7 +1463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1257,7 +1471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1265,7 +1479,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1273,7 +1487,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1281,7 +1495,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1289,7 +1503,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1297,7 +1511,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1305,7 +1519,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1313,7 +1527,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1321,7 +1535,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1329,7 +1543,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1337,7 +1551,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1345,7 +1559,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1353,7 +1567,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1361,7 +1575,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1369,7 +1583,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1377,7 +1591,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1385,7 +1599,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -1393,7 +1607,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -1401,7 +1615,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
@@ -1409,7 +1623,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>14</v>
       </c>
@@ -1417,7 +1631,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -1425,7 +1639,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
@@ -1433,7 +1647,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>14</v>
       </c>
@@ -1441,7 +1655,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
@@ -1449,7 +1663,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
@@ -1457,7 +1671,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
@@ -1465,7 +1679,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
@@ -1473,7 +1687,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
@@ -1481,7 +1695,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
@@ -1489,7 +1703,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>14</v>
       </c>
@@ -1497,7 +1711,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>14</v>
       </c>
@@ -1505,7 +1719,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
@@ -1513,7 +1727,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>14</v>
       </c>
@@ -1521,7 +1735,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>14</v>
       </c>
@@ -1529,7 +1743,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>14</v>
       </c>
@@ -1537,7 +1751,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>14</v>
       </c>
@@ -1545,7 +1759,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>14</v>
       </c>
@@ -1553,7 +1767,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>14</v>
       </c>
@@ -1561,7 +1775,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>14</v>
       </c>
@@ -1569,7 +1783,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>14</v>
       </c>
@@ -1577,7 +1791,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>14</v>
       </c>
@@ -1585,7 +1799,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -1593,7 +1807,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>14</v>
       </c>
@@ -1601,7 +1815,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>14</v>
       </c>
@@ -1609,7 +1823,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>14</v>
       </c>
@@ -1617,7 +1831,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>14</v>
       </c>
@@ -1625,7 +1839,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>58</v>
       </c>
@@ -1633,7 +1847,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>58</v>
       </c>
@@ -1641,7 +1855,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>58</v>
       </c>
@@ -1649,7 +1863,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>58</v>
       </c>
@@ -1657,7 +1871,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>58</v>
       </c>
@@ -1665,7 +1879,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>58</v>
       </c>
@@ -1673,7 +1887,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>58</v>
       </c>
@@ -1681,7 +1895,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>58</v>
       </c>
@@ -1689,7 +1903,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>58</v>
       </c>
@@ -1697,7 +1911,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>58</v>
       </c>
@@ -1705,7 +1919,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>58</v>
       </c>
@@ -1713,7 +1927,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>58</v>
       </c>
@@ -1721,7 +1935,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>58</v>
       </c>
@@ -1729,7 +1943,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>58</v>
       </c>
@@ -1737,7 +1951,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>58</v>
       </c>
@@ -1745,7 +1959,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>58</v>
       </c>
@@ -1753,7 +1967,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>58</v>
       </c>
@@ -1761,7 +1975,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>58</v>
       </c>
@@ -1769,7 +1983,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>58</v>
       </c>
@@ -1777,7 +1991,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>58</v>
       </c>
@@ -1785,7 +1999,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>58</v>
       </c>
@@ -1793,7 +2007,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>58</v>
       </c>
@@ -1801,7 +2015,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>58</v>
       </c>
@@ -1809,7 +2023,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>58</v>
       </c>
@@ -1817,7 +2031,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>58</v>
       </c>
@@ -1825,7 +2039,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>58</v>
       </c>
@@ -1833,7 +2047,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>58</v>
       </c>
@@ -1841,7 +2055,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>58</v>
       </c>
@@ -1849,7 +2063,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>58</v>
       </c>
@@ -1857,7 +2071,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>58</v>
       </c>
@@ -1865,7 +2079,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>58</v>
       </c>
@@ -1873,7 +2087,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>58</v>
       </c>
@@ -1881,7 +2095,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>58</v>
       </c>
@@ -1889,7 +2103,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>58</v>
       </c>
@@ -1897,7 +2111,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>58</v>
       </c>
@@ -1905,7 +2119,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>58</v>
       </c>
@@ -1913,7 +2127,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>58</v>
       </c>
@@ -1921,7 +2135,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>58</v>
       </c>
@@ -1929,7 +2143,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>58</v>
       </c>
@@ -1937,7 +2151,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>58</v>
       </c>
@@ -1945,7 +2159,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>58</v>
       </c>
@@ -1953,7 +2167,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>58</v>
       </c>
@@ -1961,7 +2175,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>58</v>
       </c>
@@ -1969,7 +2183,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>58</v>
       </c>
@@ -1977,7 +2191,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>58</v>
       </c>
@@ -1985,7 +2199,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>58</v>
       </c>
@@ -1993,7 +2207,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>58</v>
       </c>
@@ -2001,7 +2215,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>58</v>
       </c>
@@ -2009,7 +2223,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>58</v>
       </c>
@@ -2017,7 +2231,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>58</v>
       </c>

</xml_diff>